<commit_message>
Refactor; handle empty rows; columns
</commit_message>
<xml_diff>
--- a/spec/fixtures/column_headers.xlsx
+++ b/spec/fixtures/column_headers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emeryr/code/GIT/xlsx_to_pqc_xml/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBF636E-C504-4E41-AE9D-1F32C9140F7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFB3C97-F941-4C42-BA95-8F998BBF6320}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>ARK ID</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>0007.tif</t>
+  </si>
+  <si>
+    <t>FILLER</t>
   </si>
 </sst>
 </file>
@@ -444,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -584,6 +587,11 @@
         <v>6</v>
       </c>
     </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>